<commit_message>
more translators and testing
</commit_message>
<xml_diff>
--- a/data/published/2017_Palmer_Sauer_Holt/testInput.xlsx
+++ b/data/published/2017_Palmer_Sauer_Holt/testInput.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lauramickes/Google Drive/Current/18Modelling Programming/pyWitness/data/published/2017_Palmer_Sauer_Holt/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lauramickes/Google Drive/Current/18ModellingProgramming/pyWitness/data/published/2017_Palmer_Sauer_Holt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7623858B-362E-7446-B87D-FEFDEC0CF2FA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ACC8E15-FBFA-F241-9C1A-DC342AD13EEB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9920" yWindow="800" windowWidth="33100" windowHeight="19140" xr2:uid="{9ED41D21-AD87-EA4A-9860-FFB390C24F36}"/>
   </bookViews>
@@ -565,8 +565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D299942-CAD7-8B42-80C6-6BA1FC3BDCD5}">
   <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="117" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="117" zoomScaleNormal="117" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>